<commit_message>
Model assembly complete and display messages for hit miss and sink added
</commit_message>
<xml_diff>
--- a/excel/Ship Locations Tool.xlsx
+++ b/excel/Ship Locations Tool.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryman/Desktop/Freelance Work/Solo Coding Projects/letsplaybattleships/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{672A31F8-6E20-5E48-8745-D87C00A130EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE8EEA0-6F2F-D540-8F59-B134ED1B6E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8E89FE6B-AB32-8A4C-9463-7C5412C6025D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -606,7 +606,7 @@
   <dimension ref="B2:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,7 +618,7 @@
     <col min="5" max="5" width="13.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="10" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="10" width="10.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -638,7 +638,7 @@
     </row>
     <row r="3" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -681,7 +681,7 @@
     <row r="6" spans="2:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="str">
         <f>VLOOKUP(B3,E:F,2,0)</f>
-        <v>A0</v>
+        <v>G3</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
@@ -898,310 +898,310 @@
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E24" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E25" s="1">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G25" s="1">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E26" s="1">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G26" s="1">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E27" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G27" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E28" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E29" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G29" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E30" s="1">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G30" s="1">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E31" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G31" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E32" s="1">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G32" s="1">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E33" s="1">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G33" s="1">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E34" s="1">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G34" s="1">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E35" s="1">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G35" s="1">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E36" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G36" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E37" s="1">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G37" s="1">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E38" s="1">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G38" s="1">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E39" s="1">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G39" s="1">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E40" s="1">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G40" s="1">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E41" s="1">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G41" s="1">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E42" s="1">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G42" s="1">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E43" s="1">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G43" s="1">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E44" s="1">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G44" s="1">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E45" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G45" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E46" s="1">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G46" s="1">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E47" s="1">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G47" s="1">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E48" s="1">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G48" s="1">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E49" s="1">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G49" s="1">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E50" s="1">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G50" s="1">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E51" s="1">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G51" s="1">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added table of contents to CSS
</commit_message>
<xml_diff>
--- a/excel/Ship Locations Tool.xlsx
+++ b/excel/Ship Locations Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryman/Desktop/Freelance Work/Solo Coding Projects/letsplaybattleships/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE8EEA0-6F2F-D540-8F59-B134ED1B6E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC7C375-10A5-BA4F-BE6D-E05E1CB75E20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8E89FE6B-AB32-8A4C-9463-7C5412C6025D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Ship Location</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t xml:space="preserve">Or enter the grid reference to find the ship location value </t>
+  </si>
+  <si>
+    <t>g6</t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,7 @@
   <dimension ref="B2:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,7 +745,7 @@
     </row>
     <row r="11" spans="2:11" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1">
         <v>11</v>
@@ -785,7 +788,7 @@
     <row r="14" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <f>VLOOKUP(B11,F:G,2,0)</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1">
         <v>14</v>

</xml_diff>